<commit_message>
Added Added global V3.3 label & power BOM again
</commit_message>
<xml_diff>
--- a/Other/POWER BOM.xlsx
+++ b/Other/POWER BOM.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Desktop\EEE Stuff\EEE3088F\Project\EEE3088F-Team-9\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DE5A66-5D56-46F1-BC6C-92E92D2B5D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F95D898-C00C-4296-8AF5-A588ECDEE34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Collated Components:</t>
   </si>
@@ -190,14 +200,25 @@
   </si>
   <si>
     <t>Total cost ($)</t>
+  </si>
+  <si>
+    <t>GRAND TOTAL PER HAT ($)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -225,8 +246,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +626,10 @@
       <c r="G5">
         <v>0.01</v>
       </c>
+      <c r="H5">
+        <f>(B5*G5)</f>
+        <v>0.02</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -627,6 +653,10 @@
       <c r="G6">
         <v>0.01</v>
       </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H15" si="0">(B6*G6)</f>
+        <v>0.01</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -650,6 +680,10 @@
       <c r="G7">
         <v>0.01</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -673,6 +707,10 @@
       <c r="G8">
         <v>0.01</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -696,6 +734,10 @@
       <c r="G9">
         <v>0.01</v>
       </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -719,6 +761,10 @@
       <c r="G10">
         <v>0.02</v>
       </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -739,6 +785,13 @@
       <c r="F11" t="s">
         <v>27</v>
       </c>
+      <c r="G11">
+        <v>0.2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -759,6 +812,13 @@
       <c r="F12" t="s">
         <v>30</v>
       </c>
+      <c r="G12">
+        <v>0.01</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -779,6 +839,13 @@
       <c r="F13" t="s">
         <v>33</v>
       </c>
+      <c r="G13">
+        <v>0.2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -799,6 +866,13 @@
       <c r="F14" t="s">
         <v>36</v>
       </c>
+      <c r="G14">
+        <v>1.6</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -819,8 +893,25 @@
       <c r="F15" t="s">
         <v>39</v>
       </c>
+      <c r="G15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16">
+        <f>SUM(H5:H15)</f>
+        <v>2.3600000000000003</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>